<commit_message>
web-control update: data dir is in local web-console folder, including my.ini
</commit_message>
<xml_diff>
--- a/web-console/server/assets/excel_template.xlsx
+++ b/web-console/server/assets/excel_template.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odedkeren/dev/amicell/web-console/server/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ORA\Downloads\UBA_web\or_dev\web-console\server\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEF9A5E-1931-FF44-9AD9-D42E2F6713A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A397D30-26BD-4DAE-BDA6-F8EB98C37555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{3E3B58E4-0181-4207-8002-E1D914CEBC2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{3E3B58E4-0181-4207-8002-E1D914CEBC2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Cur" comment="all current data poitns">OFFSET(Data!$D$2,0,0,COUNTA(Data!$D:$D)-1,1)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$B$2:$K$78</definedName>
+    <definedName name="Temp">OFFSET(Data!$E$2,0,0,COUNTA(Data!$E:$E)-1,1)</definedName>
+    <definedName name="Time">OFFSET(Data!$A$2,0,0,COUNTA(Data!$A:$A)-1,1)</definedName>
+    <definedName name="Voltage" comment="the volatage data">OFFSET(Data!$C$2,0,0,COUNTA(Data!$C:$C)-1,1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Wh</t>
   </si>
@@ -129,15 +133,6 @@
     <t>Current [mA]</t>
   </si>
   <si>
-    <t>voltage [V]</t>
-  </si>
-  <si>
-    <t>timestamp [sec]</t>
-  </si>
-  <si>
-    <t>temperature [degC]</t>
-  </si>
-  <si>
     <t>Battery P.N.</t>
   </si>
   <si>
@@ -148,15 +143,40 @@
   </si>
   <si>
     <t>No. Cells in Parallel</t>
+  </si>
+  <si>
+    <t>Voltage [V]</t>
+  </si>
+  <si>
+    <t>Timestamp [sec]</t>
+  </si>
+  <si>
+    <t>Temperature [degC]</t>
+  </si>
+  <si>
+    <t>Step Type</t>
+  </si>
+  <si>
+    <t>Step Index</t>
+  </si>
+  <si>
+    <t>Plan Index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -336,49 +356,50 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -387,7 +408,26 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{BF372355-15A1-4A4A-9D8E-283F6F57B520}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{EDF64342-F5B6-40FD-AD4E-7222221C9D3C}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -423,6 +463,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Voltage</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -437,19 +480,25 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$500</c:f>
+              <c:f>[0]!Time</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="499"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$B$2:$B$500</c:f>
+              <c:f>[0]!Voltage</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="499"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -463,6 +512,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Temprture </c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -477,19 +529,25 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$500</c:f>
+              <c:f>[0]!Time</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="499"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$D$2:$D$500</c:f>
+              <c:f>[0]!Temp</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="499"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -517,6 +575,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Current</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -531,19 +592,25 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$500</c:f>
+              <c:f>[0]!Time</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="499"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$A$2:$A$500</c:f>
+              <c:f>[0]!Cur</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="499"/>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -569,7 +636,6 @@
         <c:axId val="538752176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="9000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -764,6 +830,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -771,7 +838,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1398,6 +1464,22 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD40EB8F-A777-48FF-A43D-5E9C3B26B1F8}" name="RawData" displayName="RawData" ref="A1:G2" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Normal 3" dataCellStyle="Normal 3">
+  <autoFilter ref="A1:G2" xr:uid="{BD40EB8F-A777-48FF-A43D-5E9C3B26B1F8}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{FC33533F-8141-4CC3-82AE-89F2F2B04BC6}" name="Timestamp [sec]" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{076D2A72-018C-4D9F-ACC2-105EA1D344E6}" name="Step Type" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{48324AE3-EB70-4496-95AE-5B3B594739FC}" name="Voltage [V]" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{A35D616F-7376-49EF-BD67-4E55CED9E3AB}" name="Current [mA]" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{B13C4D2C-6E24-485A-8A0D-F2AC3DB39C23}" name="Temperature [degC]" dataCellStyle="Normal 3"/>
+    <tableColumn id="6" xr3:uid="{95F8316C-CC58-4FB5-B24A-AC997E7485BE}" name="Step Index" dataCellStyle="Normal 3"/>
+    <tableColumn id="7" xr3:uid="{6D658B83-C1AC-4117-B0AF-DFEDD93C6B0F}" name="Plan Index" dataCellStyle="Normal 3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1702,27 +1784,27 @@
   </sheetPr>
   <dimension ref="B1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="2"/>
-    <col min="2" max="2" width="2.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="2.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="19.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="18"/>
-    <col min="13" max="13" width="82.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="123.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="78.83203125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.1640625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="2.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="19.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="18"/>
+    <col min="13" max="13" width="82.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="123.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="78.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1734,7 +1816,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="D3" s="7" t="s">
         <v>19</v>
@@ -1752,7 +1834,7 @@
       <c r="K3" s="9"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="2:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1765,7 +1847,7 @@
       <c r="K4" s="9"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -1777,7 +1859,7 @@
       <c r="J5" s="24"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -1789,7 +1871,7 @@
       <c r="J6" s="24"/>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -1801,7 +1883,7 @@
       <c r="J7" s="24"/>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -1813,7 +1895,7 @@
       <c r="J8" s="24"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
@@ -1825,7 +1907,7 @@
       <c r="J9" s="24"/>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -1837,7 +1919,7 @@
       <c r="J10" s="24"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -1849,7 +1931,7 @@
       <c r="J11" s="24"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -1861,7 +1943,7 @@
       <c r="J12" s="24"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
@@ -1873,7 +1955,7 @@
       <c r="J13" s="24"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
@@ -1885,7 +1967,7 @@
       <c r="J14" s="24"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
@@ -1897,7 +1979,7 @@
       <c r="J15" s="24"/>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -1909,7 +1991,7 @@
       <c r="J16" s="24"/>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
@@ -1921,7 +2003,7 @@
       <c r="J17" s="24"/>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
@@ -1933,7 +2015,7 @@
       <c r="J18" s="24"/>
       <c r="K18" s="13"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
@@ -1945,7 +2027,7 @@
       <c r="J19" s="24"/>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
@@ -1957,7 +2039,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
@@ -1969,7 +2051,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -1981,7 +2063,7 @@
       <c r="J22" s="24"/>
       <c r="K22" s="13"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
@@ -1993,7 +2075,7 @@
       <c r="J23" s="24"/>
       <c r="K23" s="13"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
@@ -2005,7 +2087,7 @@
       <c r="J24" s="24"/>
       <c r="K24" s="13"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -2017,7 +2099,7 @@
       <c r="J25" s="24"/>
       <c r="K25" s="13"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -2030,11 +2112,11 @@
       <c r="K26" s="13"/>
       <c r="M26" s="14"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="K27" s="13"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="D28" s="8" t="s">
         <v>18</v>
@@ -2051,23 +2133,23 @@
       <c r="L28" s="23"/>
       <c r="M28" s="15"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="D29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I29" s="25"/>
       <c r="K29" s="13"/>
       <c r="L29" s="23"/>
       <c r="M29" s="16"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
       <c r="H30" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I30" s="25"/>
       <c r="K30" s="13"/>
@@ -2076,7 +2158,7 @@
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="D31" s="2" t="s">
         <v>15</v>
@@ -2091,7 +2173,7 @@
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
     </row>
-    <row r="32" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="D32" s="2" t="s">
         <v>13</v>
@@ -2100,7 +2182,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="2" t="s">
@@ -2112,10 +2194,10 @@
       <c r="N32" s="17"/>
       <c r="O32" s="17"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="H33" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I33" s="25"/>
       <c r="J33" s="2" t="s">
@@ -2127,7 +2209,7 @@
       <c r="N33" s="17"/>
       <c r="O33" s="17"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
       <c r="H34" s="2" t="s">
         <v>10</v>
@@ -2142,7 +2224,7 @@
       <c r="N34" s="17"/>
       <c r="O34" s="17"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="H35" s="2" t="s">
         <v>8</v>
@@ -2154,7 +2236,7 @@
       <c r="N35" s="17"/>
       <c r="O35" s="17"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="D36" s="2" t="s">
         <v>9</v>
@@ -2169,7 +2251,7 @@
       <c r="N36" s="17"/>
       <c r="O36" s="17"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="D37" s="2" t="s">
         <v>7</v>
@@ -2184,7 +2266,7 @@
       <c r="N37" s="17"/>
       <c r="O37" s="17"/>
     </row>
-    <row r="38" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="D38" s="8" t="s">
         <v>4</v>
@@ -2195,24 +2277,24 @@
       <c r="N38" s="17"/>
       <c r="O38" s="17"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
       <c r="K39" s="13"/>
       <c r="L39" s="17"/>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
       <c r="O39" s="17"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="K40" s="13"/>
       <c r="L40" s="17"/>
@@ -2220,7 +2302,7 @@
       <c r="N40" s="17"/>
       <c r="O40" s="17"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="C41" s="2">
         <v>1</v>
@@ -2238,7 +2320,7 @@
       <c r="N41" s="17"/>
       <c r="O41" s="17"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="K42" s="13"/>
       <c r="L42" s="17"/>
@@ -2246,7 +2328,7 @@
       <c r="N42" s="17"/>
       <c r="O42" s="17"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="K43" s="13"/>
       <c r="L43" s="17"/>
@@ -2254,7 +2336,7 @@
       <c r="N43" s="17"/>
       <c r="O43" s="17"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="K44" s="13"/>
       <c r="L44" s="17"/>
@@ -2262,7 +2344,7 @@
       <c r="N44" s="17"/>
       <c r="O44" s="17"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="K45" s="13"/>
       <c r="L45" s="17"/>
@@ -2270,7 +2352,7 @@
       <c r="N45" s="17"/>
       <c r="O45" s="17"/>
     </row>
-    <row r="46" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="K46" s="13"/>
       <c r="L46" s="17"/>
@@ -2278,7 +2360,7 @@
       <c r="N46" s="17"/>
       <c r="O46" s="17"/>
     </row>
-    <row r="47" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="K47" s="13"/>
       <c r="L47" s="17"/>
@@ -2286,7 +2368,7 @@
       <c r="N47" s="17"/>
       <c r="O47" s="17"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="K48" s="13"/>
       <c r="L48" s="17"/>
@@ -2294,7 +2376,7 @@
       <c r="N48" s="17"/>
       <c r="O48" s="17"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="K49" s="13"/>
       <c r="L49" s="17"/>
@@ -2302,7 +2384,7 @@
       <c r="N49" s="17"/>
       <c r="O49" s="17"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="K50" s="13"/>
       <c r="L50" s="17"/>
@@ -2310,7 +2392,7 @@
       <c r="N50" s="17"/>
       <c r="O50" s="17"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="K51" s="13"/>
       <c r="L51" s="17"/>
@@ -2318,7 +2400,7 @@
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
       <c r="K52" s="13"/>
       <c r="L52" s="17"/>
@@ -2326,7 +2408,7 @@
       <c r="N52" s="17"/>
       <c r="O52" s="17"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
       <c r="K53" s="13"/>
       <c r="L53" s="17"/>
@@ -2334,7 +2416,7 @@
       <c r="N53" s="17"/>
       <c r="O53" s="17"/>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="12"/>
       <c r="K54" s="13"/>
       <c r="L54" s="17"/>
@@ -2342,7 +2424,7 @@
       <c r="N54" s="17"/>
       <c r="O54" s="17"/>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
       <c r="K55" s="13"/>
       <c r="L55" s="17"/>
@@ -2350,7 +2432,7 @@
       <c r="N55" s="17"/>
       <c r="O55" s="17"/>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
       <c r="K56" s="13"/>
       <c r="L56" s="17"/>
@@ -2358,7 +2440,7 @@
       <c r="N56" s="17"/>
       <c r="O56" s="17"/>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="K57" s="13"/>
       <c r="L57" s="17"/>
@@ -2366,7 +2448,7 @@
       <c r="N57" s="17"/>
       <c r="O57" s="17"/>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="K58" s="13"/>
       <c r="L58" s="17"/>
@@ -2374,7 +2456,7 @@
       <c r="N58" s="17"/>
       <c r="O58" s="17"/>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
       <c r="K59" s="13"/>
       <c r="L59" s="17"/>
@@ -2382,7 +2464,7 @@
       <c r="N59" s="17"/>
       <c r="O59" s="17"/>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" s="12"/>
       <c r="K60" s="13"/>
       <c r="L60" s="17"/>
@@ -2390,7 +2472,7 @@
       <c r="N60" s="17"/>
       <c r="O60" s="17"/>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="12"/>
       <c r="K61" s="13"/>
       <c r="L61" s="17"/>
@@ -2398,7 +2480,7 @@
       <c r="N61" s="17"/>
       <c r="O61" s="17"/>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="12"/>
       <c r="K62" s="13"/>
       <c r="L62" s="17"/>
@@ -2406,7 +2488,7 @@
       <c r="N62" s="17"/>
       <c r="O62" s="17"/>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" s="12"/>
       <c r="K63" s="13"/>
       <c r="L63" s="17"/>
@@ -2414,7 +2496,7 @@
       <c r="N63" s="17"/>
       <c r="O63" s="17"/>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
       <c r="K64" s="13"/>
       <c r="L64" s="17"/>
@@ -2422,7 +2504,7 @@
       <c r="N64" s="17"/>
       <c r="O64" s="17"/>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
       <c r="K65" s="13"/>
       <c r="L65" s="17"/>
@@ -2430,7 +2512,7 @@
       <c r="N65" s="17"/>
       <c r="O65" s="17"/>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="12"/>
       <c r="K66" s="13"/>
       <c r="L66" s="17"/>
@@ -2438,7 +2520,7 @@
       <c r="N66" s="17"/>
       <c r="O66" s="17"/>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="12"/>
       <c r="K67" s="13"/>
       <c r="L67" s="17"/>
@@ -2446,7 +2528,7 @@
       <c r="N67" s="17"/>
       <c r="O67" s="17"/>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="12"/>
       <c r="K68" s="13"/>
       <c r="L68" s="17"/>
@@ -2454,7 +2536,7 @@
       <c r="N68" s="17"/>
       <c r="O68" s="17"/>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="12"/>
       <c r="K69" s="13"/>
       <c r="L69" s="17"/>
@@ -2462,7 +2544,7 @@
       <c r="N69" s="17"/>
       <c r="O69" s="17"/>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="12"/>
       <c r="K70" s="13"/>
       <c r="L70" s="17"/>
@@ -2470,7 +2552,7 @@
       <c r="N70" s="17"/>
       <c r="O70" s="17"/>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="12"/>
       <c r="K71" s="13"/>
       <c r="L71" s="17"/>
@@ -2478,7 +2560,7 @@
       <c r="N71" s="17"/>
       <c r="O71" s="17"/>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="12"/>
       <c r="K72" s="13"/>
       <c r="L72" s="17"/>
@@ -2486,7 +2568,7 @@
       <c r="N72" s="17"/>
       <c r="O72" s="17"/>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="12"/>
       <c r="K73" s="13"/>
       <c r="L73" s="17"/>
@@ -2494,7 +2576,7 @@
       <c r="N73" s="17"/>
       <c r="O73" s="17"/>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B74" s="12"/>
       <c r="K74" s="13"/>
       <c r="L74" s="17"/>
@@ -2502,7 +2584,7 @@
       <c r="N74" s="17"/>
       <c r="O74" s="17"/>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75" s="12"/>
       <c r="K75" s="13"/>
       <c r="L75" s="17"/>
@@ -2510,7 +2592,7 @@
       <c r="N75" s="17"/>
       <c r="O75" s="17"/>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="12"/>
       <c r="K76" s="13"/>
       <c r="L76" s="17"/>
@@ -2518,7 +2600,7 @@
       <c r="N76" s="17"/>
       <c r="O76" s="17"/>
     </row>
-    <row r="77" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="19"/>
       <c r="C77" s="20"/>
       <c r="D77" s="20"/>
@@ -2532,7 +2614,7 @@
       <c r="L77" s="23"/>
       <c r="M77" s="22"/>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
@@ -2549,34 +2631,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE78AA8-3E87-47A3-991D-56AC1DEC39E3}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="16.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="76" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="E1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>